<commit_message>
feat: presigned_url이 아닌 download_key를 넘기도록 수정
- CORS 문제 때문에, url 말고 key를 넘겨 다운할 수 있도록 함
- /download/{file_key}로 응답 받은 key를 담아 요청을 보내면 바로 다운로드 가능
</commit_message>
<xml_diff>
--- a/backend/agent-service/app/services/code_gen/test.xlsx
+++ b/backend/agent-service/app/services/code_gen/test.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$5:$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$5:$L$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,21 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>안녕하세요 템플릿입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>막 들어있고</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이렇게</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기존 컬럼들이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -72,14 +60,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2열 5행에</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>여기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아래에</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -97,6 +77,34 @@
   </si>
   <si>
     <t>거에요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기존</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컬럼들이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이렇게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>막</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>들어있고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1열 5행에</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -765,69 +773,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J164"/>
+  <dimension ref="A1:L164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="14.4140625" style="18" customWidth="1"/>
-    <col min="11" max="14" width="8.6640625" style="18"/>
-    <col min="15" max="15" width="13.08203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.08203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5" style="18" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="18"/>
+    <col min="2" max="12" width="14.4140625" style="18" customWidth="1"/>
+    <col min="13" max="16" width="8.6640625" style="18"/>
+    <col min="17" max="17" width="13.08203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="11.08203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.6640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="10"/>
       <c r="B1" s="11" t="str">
         <f>B5</f>
-        <v>기존 컬럼들이</v>
+        <v>기존</v>
       </c>
       <c r="C1" s="11" t="str">
-        <f t="shared" ref="C1:J1" si="0">C5</f>
-        <v>이렇게</v>
+        <f t="shared" ref="C1:L1" si="0">C5</f>
+        <v>컬럼들이</v>
       </c>
       <c r="D1" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>막 들어있고</v>
+        <v>이렇게</v>
       </c>
       <c r="E1" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>여기</v>
+        <v>막</v>
       </c>
       <c r="F1" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>아래에</v>
+        <v>들어있고</v>
       </c>
       <c r="G1" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>내</v>
+        <v>여기</v>
       </c>
       <c r="H1" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>데이터를</v>
+        <v>아래에</v>
       </c>
       <c r="I1" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>붙일</v>
+        <v>내</v>
       </c>
       <c r="J1" s="11" t="str">
         <f t="shared" si="0"/>
+        <v>데이터를</v>
+      </c>
+      <c r="K1" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>붙일</v>
+      </c>
+      <c r="L1" s="11" t="str">
+        <f t="shared" si="0"/>
         <v>거에요</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="13">
-        <f t="shared" ref="B2:J2" si="1">SUM(B6:B164)</f>
+        <f t="shared" ref="B2:L2" si="1">SUM(B6:B164)</f>
         <v>0</v>
       </c>
       <c r="C2" s="13">
@@ -858,14 +874,22 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="K2" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L2" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
@@ -875,44 +899,52 @@
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+    </row>
+    <row r="4" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="15" t="s">
         <v>1</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
-        <v>4</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -922,11 +954,13 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -936,11 +970,13 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -950,11 +986,13 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -964,11 +1002,13 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -978,11 +1018,13 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -992,11 +1034,13 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1006,9 +1050,11 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1018,9 +1064,11 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1030,9 +1078,11 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1042,9 +1092,11 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1054,9 +1106,11 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="16"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1066,9 +1120,11 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="16"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1078,9 +1134,11 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="16"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1090,9 +1148,11 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="16"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1102,9 +1162,11 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="16"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1114,9 +1176,11 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="16"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1126,9 +1190,11 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="16"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1138,9 +1204,11 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="16"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1150,9 +1218,11 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="16"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1162,9 +1232,11 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="4"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="16"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1174,9 +1246,11 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="16"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1186,9 +1260,11 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="4"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="16"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1198,9 +1274,11 @@
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="16"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1210,9 +1288,11 @@
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="16"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1222,9 +1302,11 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="4"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="16"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1234,9 +1316,11 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="16"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1246,9 +1330,11 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="16"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1258,9 +1344,11 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="4"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="16"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1270,9 +1358,11 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="16"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1282,9 +1372,11 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="4"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" s="16"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1294,9 +1386,11 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="4"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="16"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1306,9 +1400,11 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="16"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1318,9 +1414,11 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="4"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="16"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1330,9 +1428,11 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="16"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1342,9 +1442,11 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="16"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1354,9 +1456,11 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="16"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1366,9 +1470,11 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="16"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1378,9 +1484,11 @@
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" s="16"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1390,9 +1498,11 @@
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
-      <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" s="16"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1402,9 +1512,11 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
-      <c r="J45" s="4"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="16"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1414,9 +1526,11 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
-      <c r="J46" s="4"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="16"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1426,9 +1540,11 @@
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="4"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A48" s="16"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1438,9 +1554,11 @@
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="4"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="16"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1450,9 +1568,11 @@
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="4"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="16"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1462,9 +1582,11 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="J50" s="4"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="16"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1474,9 +1596,11 @@
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
-      <c r="J51" s="4"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="16"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1486,9 +1610,11 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
-      <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="16"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1498,9 +1624,11 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-      <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="16"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1510,9 +1638,11 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
-      <c r="J54" s="4"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="16"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1522,9 +1652,11 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
-      <c r="J55" s="4"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="16"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1534,9 +1666,11 @@
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
-      <c r="J56" s="4"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="16"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1546,9 +1680,11 @@
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
-      <c r="J57" s="4"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="16"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1558,9 +1694,11 @@
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
-      <c r="J58" s="4"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="4"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" s="16"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1570,9 +1708,11 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
-      <c r="J59" s="4"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="4"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="16"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1582,9 +1722,11 @@
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
-      <c r="J60" s="4"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" s="16"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1594,9 +1736,11 @@
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
-      <c r="J61" s="4"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" s="16"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1606,9 +1750,11 @@
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="16"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1618,9 +1764,11 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
-      <c r="J63" s="4"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="16"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1630,9 +1778,11 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
-      <c r="J64" s="4"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A65" s="16"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1642,9 +1792,11 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
-      <c r="J65" s="4"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="4"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A66" s="16"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1654,9 +1806,11 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
-      <c r="J66" s="4"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67" s="16"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1666,9 +1820,11 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
-      <c r="J67" s="4"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="4"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A68" s="16"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1678,9 +1834,11 @@
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
-      <c r="J68" s="4"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="4"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69" s="16"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1690,9 +1848,11 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
-      <c r="J69" s="4"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="4"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70" s="16"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1702,9 +1862,11 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
-      <c r="J70" s="4"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="4"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" s="16"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1714,9 +1876,11 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
-      <c r="J71" s="4"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72" s="16"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1726,9 +1890,11 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
-      <c r="J72" s="4"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="4"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" s="16"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1738,9 +1904,11 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
-      <c r="J73" s="4"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="4"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="16"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1750,9 +1918,11 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
-      <c r="J74" s="4"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="4"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" s="16"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1762,9 +1932,11 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
-      <c r="J75" s="4"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="4"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" s="16"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1774,9 +1946,11 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
-      <c r="J76" s="4"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="4"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" s="16"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1786,9 +1960,11 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
-      <c r="J77" s="4"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="4"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" s="16"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1798,9 +1974,11 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
-      <c r="J78" s="4"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="4"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79" s="16"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -1810,9 +1988,11 @@
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
-      <c r="J79" s="4"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="4"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" s="16"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -1822,9 +2002,11 @@
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
-      <c r="J80" s="4"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="4"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" s="16"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -1834,9 +2016,11 @@
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="4"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="4"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" s="16"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -1846,9 +2030,11 @@
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-      <c r="J82" s="4"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="4"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" s="16"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -1858,9 +2044,11 @@
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="J83" s="4"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="4"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" s="16"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -1870,9 +2058,11 @@
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
-      <c r="J84" s="4"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="4"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" s="16"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -1882,9 +2072,11 @@
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
-      <c r="J85" s="4"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="4"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" s="16"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -1894,9 +2086,11 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
-      <c r="J86" s="4"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="4"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="16"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -1906,9 +2100,11 @@
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
-      <c r="J87" s="4"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="4"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88" s="16"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -1918,9 +2114,11 @@
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-      <c r="J88" s="4"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="4"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89" s="16"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -1930,9 +2128,11 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-      <c r="J89" s="4"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="4"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90" s="16"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -1942,9 +2142,11 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-      <c r="J90" s="4"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="4"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" s="16"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -1954,9 +2156,11 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
-      <c r="J91" s="4"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="4"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92" s="16"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -1966,9 +2170,11 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="4"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="4"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A93" s="16"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -1978,9 +2184,11 @@
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="J93" s="4"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="4"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A94" s="16"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -1990,9 +2198,11 @@
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-      <c r="J94" s="4"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="4"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A95" s="16"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2002,9 +2212,11 @@
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-      <c r="J95" s="4"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="4"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A96" s="16"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -2014,9 +2226,11 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="4"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="4"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A97" s="16"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -2026,9 +2240,11 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
-      <c r="J97" s="4"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="4"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A98" s="16"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -2038,9 +2254,11 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="4"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="4"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A99" s="16"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -2050,9 +2268,11 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
-      <c r="J99" s="4"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="4"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A100" s="16"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -2062,9 +2282,11 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
-      <c r="J100" s="4"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="4"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A101" s="16"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -2074,9 +2296,11 @@
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
-      <c r="J101" s="4"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="4"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102" s="16"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -2086,9 +2310,11 @@
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
-      <c r="J102" s="4"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="4"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" s="16"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2098,9 +2324,11 @@
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-      <c r="J103" s="4"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="4"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" s="16"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -2110,9 +2338,11 @@
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="4"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="4"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" s="16"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -2122,9 +2352,11 @@
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-      <c r="J105" s="4"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="4"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" s="16"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -2134,9 +2366,11 @@
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
-      <c r="J106" s="4"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="4"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" s="16"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -2146,9 +2380,11 @@
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-      <c r="J107" s="4"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="4"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A108" s="16"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -2158,9 +2394,11 @@
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
-      <c r="J108" s="4"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J108" s="3"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="4"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109" s="16"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -2170,9 +2408,11 @@
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-      <c r="J109" s="4"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="4"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110" s="16"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -2182,9 +2422,11 @@
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
-      <c r="J110" s="4"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J110" s="3"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="4"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A111" s="16"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -2194,9 +2436,11 @@
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
-      <c r="J111" s="4"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="4"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A112" s="16"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -2206,9 +2450,11 @@
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
-      <c r="J112" s="4"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="4"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A113" s="16"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -2218,9 +2464,11 @@
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-      <c r="J113" s="4"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J113" s="3"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="4"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A114" s="16"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -2230,9 +2478,11 @@
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-      <c r="J114" s="4"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J114" s="3"/>
+      <c r="K114" s="3"/>
+      <c r="L114" s="4"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A115" s="16"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -2242,9 +2492,11 @@
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
-      <c r="J115" s="4"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="4"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A116" s="16"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -2254,9 +2506,11 @@
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
-      <c r="J116" s="4"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="4"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A117" s="16"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -2266,9 +2520,11 @@
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
-      <c r="J117" s="4"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J117" s="3"/>
+      <c r="K117" s="3"/>
+      <c r="L117" s="4"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A118" s="16"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -2278,9 +2534,11 @@
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
-      <c r="J118" s="4"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="4"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A119" s="16"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -2290,9 +2548,11 @@
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
-      <c r="J119" s="4"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J119" s="3"/>
+      <c r="K119" s="3"/>
+      <c r="L119" s="4"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A120" s="16"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -2302,9 +2562,11 @@
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
-      <c r="J120" s="4"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="4"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A121" s="16"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -2314,9 +2576,11 @@
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
-      <c r="J121" s="4"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J121" s="3"/>
+      <c r="K121" s="3"/>
+      <c r="L121" s="4"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A122" s="16"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -2326,9 +2590,11 @@
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
-      <c r="J122" s="4"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="4"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A123" s="16"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -2338,9 +2604,11 @@
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
-      <c r="J123" s="4"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J123" s="3"/>
+      <c r="K123" s="3"/>
+      <c r="L123" s="4"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A124" s="16"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -2350,9 +2618,11 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
-      <c r="J124" s="4"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="4"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A125" s="16"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -2362,9 +2632,11 @@
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
-      <c r="J125" s="4"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J125" s="3"/>
+      <c r="K125" s="3"/>
+      <c r="L125" s="4"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A126" s="16"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -2374,9 +2646,11 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-      <c r="J126" s="4"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="4"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A127" s="16"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -2386,9 +2660,11 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-      <c r="J127" s="4"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J127" s="3"/>
+      <c r="K127" s="3"/>
+      <c r="L127" s="4"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A128" s="16"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -2398,9 +2674,11 @@
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
-      <c r="J128" s="4"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="4"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A129" s="16"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2410,9 +2688,11 @@
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
-      <c r="J129" s="4"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J129" s="3"/>
+      <c r="K129" s="3"/>
+      <c r="L129" s="4"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A130" s="16"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2422,9 +2702,11 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
-      <c r="J130" s="4"/>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="4"/>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A131" s="16"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -2434,9 +2716,11 @@
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
-      <c r="J131" s="4"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+      <c r="L131" s="4"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A132" s="16"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -2446,9 +2730,11 @@
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
-      <c r="J132" s="4"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="4"/>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A133" s="16"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -2458,9 +2744,11 @@
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
-      <c r="J133" s="4"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J133" s="3"/>
+      <c r="K133" s="3"/>
+      <c r="L133" s="4"/>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A134" s="16"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -2470,9 +2758,11 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
-      <c r="J134" s="4"/>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="4"/>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A135" s="16"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -2482,9 +2772,11 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
-      <c r="J135" s="4"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="4"/>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A136" s="16"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -2494,9 +2786,11 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
-      <c r="J136" s="4"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="4"/>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A137" s="16"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -2506,9 +2800,11 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
-      <c r="J137" s="4"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="4"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A138" s="16"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -2518,9 +2814,11 @@
       <c r="G138" s="3"/>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
-      <c r="J138" s="4"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="4"/>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A139" s="16"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -2530,9 +2828,11 @@
       <c r="G139" s="3"/>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
-      <c r="J139" s="4"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J139" s="3"/>
+      <c r="K139" s="3"/>
+      <c r="L139" s="4"/>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A140" s="16"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -2542,9 +2842,11 @@
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
-      <c r="J140" s="4"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="4"/>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A141" s="16"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -2554,9 +2856,11 @@
       <c r="G141" s="3"/>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
-      <c r="J141" s="4"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J141" s="3"/>
+      <c r="K141" s="3"/>
+      <c r="L141" s="4"/>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A142" s="16"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -2566,9 +2870,11 @@
       <c r="G142" s="3"/>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
-      <c r="J142" s="4"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="4"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A143" s="16"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -2578,9 +2884,11 @@
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
-      <c r="J143" s="4"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J143" s="3"/>
+      <c r="K143" s="3"/>
+      <c r="L143" s="4"/>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A144" s="16"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -2590,9 +2898,11 @@
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
-      <c r="J144" s="4"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="4"/>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A145" s="16"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -2602,9 +2912,11 @@
       <c r="G145" s="3"/>
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
-      <c r="J145" s="4"/>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="4"/>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A146" s="16"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -2614,9 +2926,11 @@
       <c r="G146" s="3"/>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
-      <c r="J146" s="4"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="4"/>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A147" s="16"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -2626,9 +2940,11 @@
       <c r="G147" s="3"/>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
-      <c r="J147" s="4"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="4"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A148" s="16"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -2638,9 +2954,11 @@
       <c r="G148" s="3"/>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>
-      <c r="J148" s="4"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="4"/>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A149" s="16"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -2650,9 +2968,11 @@
       <c r="G149" s="3"/>
       <c r="H149" s="3"/>
       <c r="I149" s="3"/>
-      <c r="J149" s="4"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="4"/>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A150" s="16"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -2662,9 +2982,11 @@
       <c r="G150" s="3"/>
       <c r="H150" s="3"/>
       <c r="I150" s="3"/>
-      <c r="J150" s="4"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="4"/>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A151" s="16"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -2674,9 +2996,11 @@
       <c r="G151" s="3"/>
       <c r="H151" s="3"/>
       <c r="I151" s="3"/>
-      <c r="J151" s="4"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J151" s="3"/>
+      <c r="K151" s="3"/>
+      <c r="L151" s="4"/>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A152" s="16"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -2686,9 +3010,11 @@
       <c r="G152" s="3"/>
       <c r="H152" s="3"/>
       <c r="I152" s="3"/>
-      <c r="J152" s="4"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+      <c r="L152" s="4"/>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A153" s="16"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -2698,9 +3024,11 @@
       <c r="G153" s="3"/>
       <c r="H153" s="3"/>
       <c r="I153" s="3"/>
-      <c r="J153" s="4"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J153" s="3"/>
+      <c r="K153" s="3"/>
+      <c r="L153" s="4"/>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A154" s="16"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -2710,9 +3038,11 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
-      <c r="J154" s="4"/>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J154" s="3"/>
+      <c r="K154" s="3"/>
+      <c r="L154" s="4"/>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A155" s="16"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -2722,9 +3052,11 @@
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
-      <c r="J155" s="4"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J155" s="3"/>
+      <c r="K155" s="3"/>
+      <c r="L155" s="4"/>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A156" s="16"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -2734,9 +3066,11 @@
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
-      <c r="J156" s="4"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J156" s="3"/>
+      <c r="K156" s="3"/>
+      <c r="L156" s="4"/>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A157" s="16"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -2746,9 +3080,11 @@
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
-      <c r="J157" s="4"/>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J157" s="3"/>
+      <c r="K157" s="3"/>
+      <c r="L157" s="4"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A158" s="16"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -2758,9 +3094,11 @@
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
-      <c r="J158" s="4"/>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J158" s="3"/>
+      <c r="K158" s="3"/>
+      <c r="L158" s="4"/>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A159" s="16"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -2770,9 +3108,11 @@
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
-      <c r="J159" s="4"/>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J159" s="3"/>
+      <c r="K159" s="3"/>
+      <c r="L159" s="4"/>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A160" s="16"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -2782,9 +3122,11 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
-      <c r="J160" s="4"/>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="4"/>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A161" s="16"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
@@ -2794,9 +3136,11 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
-      <c r="J161" s="4"/>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J161" s="3"/>
+      <c r="K161" s="3"/>
+      <c r="L161" s="4"/>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A162" s="16"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
@@ -2806,9 +3150,11 @@
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
-      <c r="J162" s="4"/>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J162" s="3"/>
+      <c r="K162" s="3"/>
+      <c r="L162" s="4"/>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A163" s="16"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -2818,9 +3164,11 @@
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
-      <c r="J163" s="4"/>
-    </row>
-    <row r="164" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="4"/>
+    </row>
+    <row r="164" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A164" s="17"/>
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
@@ -2830,10 +3178,12 @@
       <c r="G164" s="5"/>
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
-      <c r="J164" s="6"/>
+      <c r="J164" s="5"/>
+      <c r="K164" s="5"/>
+      <c r="L164" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:J5">
+  <autoFilter ref="B5:L5">
     <sortState ref="B6:J12">
       <sortCondition ref="B5"/>
     </sortState>
@@ -2842,7 +3192,7 @@
     <sortCondition ref="B5"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>